<commit_message>
Cambio de parametros en EE
</commit_message>
<xml_diff>
--- a/data/EEParams2.xlsx
+++ b/data/EEParams2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="4980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="4980" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="costoVacuna" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +145,14 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,8 +171,14 @@
         <bgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,6 +191,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -198,9 +225,13 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1505,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -4070,7 +4101,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4079,7 +4112,7 @@
     <col min="3" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -4090,539 +4123,539 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="11">
+        <v>116.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="11">
         <v>130.05000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="11">
         <v>262.94</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="11">
         <v>239.22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="10">
-        <v>100.23042316258349</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="11">
+        <v>105.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="11">
         <v>25.93</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="11">
         <v>251.2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="11">
         <v>236.38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="10">
-        <v>147.34216035634745</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="11">
+        <v>166.81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="11">
         <v>159.08000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="11">
         <v>199.73</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="11">
         <v>191.28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="10">
-        <v>168.27487750556793</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="11">
+        <v>179.55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="11">
         <v>213.19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="11">
         <v>408.85</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="11">
         <v>397.79</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="10">
-        <v>110.80570155902004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="11">
+        <v>150.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="11">
         <v>444.49</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="11">
         <v>2368.19</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="11">
         <v>2116.56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="10">
-        <v>190.47652561247213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="11">
+        <v>195.62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="11">
         <v>224.63</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="11">
         <v>384.23</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="11">
         <v>366.74</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="11">
         <v>0.45</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="11">
         <v>0.71</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+        <v>147.06</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C46" s="12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="11" t="s">
+        <v>127.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="12">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="11" t="s">
+        <v>377.12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C48" s="12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
+        <v>356.13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="12">
         <v>0.45</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="11" t="s">
+    <row r="50" spans="1:3" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="12">
@@ -5581,6 +5614,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>